<commit_message>
add some test case
</commit_message>
<xml_diff>
--- a/docs/issues/jarvis2-issue-schedule.xlsx
+++ b/docs/issues/jarvis2-issue-schedule.xlsx
@@ -2340,7 +2340,7 @@
     <col min="3" max="3" width="38.7109" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.53906" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.2812" style="1" customWidth="1"/>
     <col min="7" max="7" width="6.75" style="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="1" customWidth="1"/>
@@ -5710,7 +5710,7 @@
         <v>14</v>
       </c>
       <c r="J111" t="s" s="5">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="K111" s="7">
         <v>16</v>
@@ -7846,8 +7846,12 @@
       <c r="E182" t="s" s="5">
         <v>213</v>
       </c>
-      <c r="F182" s="5"/>
-      <c r="G182" s="7"/>
+      <c r="F182" t="s" s="5">
+        <v>58</v>
+      </c>
+      <c r="G182" t="s" s="5">
+        <v>12</v>
+      </c>
       <c r="H182" t="s" s="5">
         <v>25</v>
       </c>
@@ -8388,7 +8392,7 @@
       <c r="J203" s="7"/>
       <c r="K203" s="7">
         <f>SUMIFS(K1:K200,G1:G200,"&lt;&gt;close",J1:J200,"=alpha")</f>
-        <v>453</v>
+        <v>429</v>
       </c>
       <c r="L203" s="7"/>
       <c r="M203" s="4"/>

</xml_diff>